<commit_message>
Update test case: Address Reference (1)
</commit_message>
<xml_diff>
--- a/System 6 Renovation Working Files/Test Files/Address Reference (1).xlsx
+++ b/System 6 Renovation Working Files/Test Files/Address Reference (1).xlsx
@@ -6239,8 +6239,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:HV1187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GT1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="HA5" sqref="HA5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>